<commit_message>
update cleanv3 file. add science plot formatter
</commit_message>
<xml_diff>
--- a/examples/python/lasso_and_n4sid/n4sid_v6/output/u1test_tvps.xlsx
+++ b/examples/python/lasso_and_n4sid/n4sid_v6/output/u1test_tvps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/controls/MODRLC-StateEstimation/examples/python/lasso_and_n4sid/n4sid_v6/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36AF5BE-4A84-AF4E-BD0E-4ADD061DF77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B7D65C-9C9A-5F4D-8CE4-84763F1C593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40840" windowHeight="28340" xr2:uid="{188B36D1-0417-0F4E-BAF5-A32276AFD9EA}"/>
   </bookViews>
@@ -18674,7 +18674,7 @@
   <dimension ref="A1:G1441"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="E1" activeCellId="2" sqref="C1:C1048576 F1:F1048576 E1:E1048576"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>